<commit_message>
Añado ficheros del Minint
</commit_message>
<xml_diff>
--- a/Partidos2019.xlsx
+++ b/Partidos2019.xlsx
@@ -5,10 +5,10 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\HONDT\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\dHondt\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B073FBAC-39AE-4765-9692-ECBF3CA4F9FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{E5473D0E-DD02-44F0-B0A4-EBA7B3271D2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11760" xr2:uid="{59EF6071-CF02-452A-AEA2-E4489B6EE2E3}"/>
   </bookViews>
@@ -282,12 +282,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -606,7 +605,7 @@
   <dimension ref="A1:BO3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -666,7 +665,7 @@
     <col min="67" max="67" width="7" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:67" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A1" s="1">
         <v>1</v>
       </c>

</xml_diff>